<commit_message>
added team spec time commit pt2
</commit_message>
<xml_diff>
--- a/team_specific_matrix/Penn_A.xlsx
+++ b/team_specific_matrix/Penn_A.xlsx
@@ -498,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1953255425709516</v>
+        <v>0.196078431372549</v>
       </c>
       <c r="C2">
-        <v>0.5492487479131887</v>
+        <v>0.5490196078431373</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -522,7 +522,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.01168614357262104</v>
+        <v>0.01143790849673203</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -537,10 +537,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0.001669449081803005</v>
+        <v>0.001633986928104575</v>
       </c>
       <c r="P2">
-        <v>0.1452420701168614</v>
+        <v>0.1470588235294118</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -549,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0.09682804674457429</v>
+        <v>0.09477124183006536</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -557,10 +557,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.01685393258426966</v>
+        <v>0.01652892561983471</v>
       </c>
       <c r="C3">
-        <v>0.06741573033707865</v>
+        <v>0.06611570247933884</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.008426966292134831</v>
+        <v>0.008264462809917356</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.7191011235955056</v>
+        <v>0.721763085399449</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0.1882022471910112</v>
+        <v>0.1873278236914601</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.03947368421052631</v>
+        <v>0.03896103896103896</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.6052631578947368</v>
+        <v>0.6103896103896104</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.3552631578947368</v>
+        <v>0.3506493506493507</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -734,19 +734,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.07390300230946882</v>
+        <v>0.07317073170731707</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.002309468822170901</v>
+        <v>0.002217294900221729</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.06697459584295612</v>
+        <v>0.06651884700665188</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.2448036951501155</v>
+        <v>0.2483370288248337</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -773,19 +773,19 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.0207852193995381</v>
+        <v>0.01995565410199556</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.1547344110854504</v>
+        <v>0.1552106430155211</v>
       </c>
       <c r="R6">
-        <v>0.07621247113163972</v>
+        <v>0.07760532150776053</v>
       </c>
       <c r="S6">
-        <v>0.3602771362586605</v>
+        <v>0.3569844789356985</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -793,19 +793,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.1143617021276596</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.02127659574468085</v>
+        <v>0.0202020202020202</v>
       </c>
       <c r="E7">
-        <v>0.002659574468085106</v>
+        <v>0.002525252525252525</v>
       </c>
       <c r="F7">
-        <v>0.05851063829787234</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.125</v>
+        <v>0.1237373737373737</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -832,19 +832,19 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0.01861702127659574</v>
+        <v>0.01767676767676768</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0.1914893617021277</v>
+        <v>0.1868686868686869</v>
       </c>
       <c r="R7">
-        <v>0.09574468085106383</v>
+        <v>0.101010101010101</v>
       </c>
       <c r="S7">
-        <v>0.3723404255319149</v>
+        <v>0.3813131313131313</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -852,19 +852,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.09154228855721393</v>
+        <v>0.09117361784675072</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.01691542288557214</v>
+        <v>0.01745877788554801</v>
       </c>
       <c r="E8">
-        <v>0.0009950248756218905</v>
+        <v>0.0009699321047526673</v>
       </c>
       <c r="F8">
-        <v>0.05970149253731343</v>
+        <v>0.05819592628516004</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.1134328358208955</v>
+        <v>0.1134820562560621</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -891,19 +891,19 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0.01592039800995025</v>
+        <v>0.01551891367604268</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0.173134328358209</v>
+        <v>0.1726479146459748</v>
       </c>
       <c r="R8">
-        <v>0.09751243781094528</v>
+        <v>0.09990300678952474</v>
       </c>
       <c r="S8">
-        <v>0.4308457711442786</v>
+        <v>0.4306498545101843</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -911,19 +911,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.09382151029748284</v>
+        <v>0.09429824561403509</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.009153318077803204</v>
+        <v>0.008771929824561403</v>
       </c>
       <c r="E9">
-        <v>0.002288329519450801</v>
+        <v>0.002192982456140351</v>
       </c>
       <c r="F9">
-        <v>0.06178489702517163</v>
+        <v>0.06140350877192982</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.1098398169336384</v>
+        <v>0.1074561403508772</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -950,19 +950,19 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0.0137299771167048</v>
+        <v>0.01535087719298246</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0.1510297482837529</v>
+        <v>0.1513157894736842</v>
       </c>
       <c r="R9">
-        <v>0.09610983981693363</v>
+        <v>0.09429824561403509</v>
       </c>
       <c r="S9">
-        <v>0.4622425629290618</v>
+        <v>0.4649122807017544</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -970,19 +970,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1011673151750973</v>
+        <v>0.09939759036144578</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.01828793774319066</v>
+        <v>0.01769578313253012</v>
       </c>
       <c r="E10">
-        <v>0.002334630350194552</v>
+        <v>0.002259036144578313</v>
       </c>
       <c r="F10">
-        <v>0.0669260700389105</v>
+        <v>0.06890060240963855</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.111284046692607</v>
+        <v>0.1118222891566265</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1009,19 +1009,19 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0.01439688715953307</v>
+        <v>0.01393072289156626</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0.198443579766537</v>
+        <v>0.1976656626506024</v>
       </c>
       <c r="R10">
-        <v>0.08949416342412451</v>
+        <v>0.09186746987951808</v>
       </c>
       <c r="S10">
-        <v>0.3976653696498054</v>
+        <v>0.396460843373494</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.1441441441441441</v>
+        <v>0.1416234887737478</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1053,13 +1053,13 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.08468468468468468</v>
+        <v>0.08117443868739206</v>
       </c>
       <c r="K11">
-        <v>0.2036036036036036</v>
+        <v>0.1986183074265976</v>
       </c>
       <c r="L11">
-        <v>0.5513513513513514</v>
+        <v>0.5630397236614854</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1080,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0.01621621621621622</v>
+        <v>0.0155440414507772</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.7508090614886731</v>
+        <v>0.7492447129909365</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1112,13 +1112,13 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.1812297734627832</v>
+        <v>0.1812688821752266</v>
       </c>
       <c r="K12">
-        <v>0.003236245954692557</v>
+        <v>0.003021148036253776</v>
       </c>
       <c r="L12">
-        <v>0.02588996763754045</v>
+        <v>0.03021148036253777</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0.03883495145631068</v>
+        <v>0.03625377643504532</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.7184466019417476</v>
+        <v>0.7169811320754716</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.2233009708737864</v>
+        <v>0.2264150943396226</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0.05825242718446602</v>
+        <v>0.05660377358490566</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1277,34 +1277,34 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.018140589569161</v>
+        <v>0.01762114537444934</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.1564625850340136</v>
+        <v>0.1585903083700441</v>
       </c>
       <c r="I15">
-        <v>0.08843537414965986</v>
+        <v>0.0881057268722467</v>
       </c>
       <c r="J15">
-        <v>0.3718820861678004</v>
+        <v>0.3744493392070485</v>
       </c>
       <c r="K15">
-        <v>0.036281179138322</v>
+        <v>0.03524229074889868</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0.01133786848072562</v>
+        <v>0.013215859030837</v>
       </c>
       <c r="N15">
-        <v>0.002267573696145125</v>
+        <v>0.002202643171806168</v>
       </c>
       <c r="O15">
-        <v>0.06122448979591837</v>
+        <v>0.05947136563876652</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0.253968253968254</v>
+        <v>0.2511013215859031</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1336,34 +1336,34 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.01827676240208877</v>
+        <v>0.0178117048346056</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.1566579634464752</v>
+        <v>0.1552162849872774</v>
       </c>
       <c r="I16">
-        <v>0.06788511749347259</v>
+        <v>0.06870229007633588</v>
       </c>
       <c r="J16">
-        <v>0.4490861618798956</v>
+        <v>0.4478371501272265</v>
       </c>
       <c r="K16">
-        <v>0.09921671018276762</v>
+        <v>0.09923664122137404</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0.02349869451697128</v>
+        <v>0.02290076335877863</v>
       </c>
       <c r="N16">
-        <v>0.005221932114882507</v>
+        <v>0.005089058524173028</v>
       </c>
       <c r="O16">
-        <v>0.04699738903394256</v>
+        <v>0.04580152671755725</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0.1331592689295039</v>
+        <v>0.1374045801526718</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1395,34 +1395,34 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.01240135287485907</v>
+        <v>0.01203501094091904</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0.1927846674182638</v>
+        <v>0.1892778993435449</v>
       </c>
       <c r="I17">
-        <v>0.1071025930101466</v>
+        <v>0.1072210065645514</v>
       </c>
       <c r="J17">
-        <v>0.3945885005636979</v>
+        <v>0.3982494529540481</v>
       </c>
       <c r="K17">
-        <v>0.09582863585118377</v>
+        <v>0.0962800875273523</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0.01578354002254791</v>
+        <v>0.01531728665207877</v>
       </c>
       <c r="N17">
-        <v>0.00112739571589628</v>
+        <v>0.001094091903719912</v>
       </c>
       <c r="O17">
-        <v>0.06313416009019165</v>
+        <v>0.06236323851203501</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0.1172491544532131</v>
+        <v>0.1181619256017506</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1454,34 +1454,34 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.01136363636363636</v>
+        <v>0.0128755364806867</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.1863636363636364</v>
+        <v>0.1802575107296137</v>
       </c>
       <c r="I18">
-        <v>0.09545454545454546</v>
+        <v>0.09012875536480687</v>
       </c>
       <c r="J18">
-        <v>0.4318181818181818</v>
+        <v>0.4248927038626609</v>
       </c>
       <c r="K18">
-        <v>0.07954545454545454</v>
+        <v>0.08798283261802575</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0.02045454545454545</v>
+        <v>0.01931330472103004</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0.06818181818181818</v>
+        <v>0.06866952789699571</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0.1068181818181818</v>
+        <v>0.1158798283261803</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1513,34 +1513,34 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0.01639941690962099</v>
+        <v>0.01658433309809457</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0.228134110787172</v>
+        <v>0.2275935074100212</v>
       </c>
       <c r="I19">
-        <v>0.08782798833819241</v>
+        <v>0.08997882851093861</v>
       </c>
       <c r="J19">
-        <v>0.3618804664723032</v>
+        <v>0.3599153140437544</v>
       </c>
       <c r="K19">
-        <v>0.09438775510204081</v>
+        <v>0.09562455892731123</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0.02551020408163265</v>
+        <v>0.02540578687367678</v>
       </c>
       <c r="N19">
-        <v>0.0003644314868804665</v>
+        <v>0.0003528581510232887</v>
       </c>
       <c r="O19">
-        <v>0.06523323615160349</v>
+        <v>0.06563161609033169</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -1552,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>0.1202623906705539</v>
+        <v>0.1189131968948483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>